<commit_message>
add simple health properties from spreadsheet
</commit_message>
<xml_diff>
--- a/services/health/cloud-mesh-security-use-case-table.xlsx
+++ b/services/health/cloud-mesh-security-use-case-table.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="29005"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\underwood\gov\NIST\Big Data\big data security\Gregor Cloud Mesh collaboration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grey/github/cloudmesh-community/nist/services/health/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16710" windowHeight="7980"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="6" r:id="rId1"/>
@@ -20,9 +20,15 @@
     <sheet name="Version History" sheetId="3" r:id="rId6"/>
     <sheet name="Bibliography" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="194">
   <si>
     <t>Object</t>
   </si>
@@ -585,12 +591,39 @@
   </si>
   <si>
     <t>ZigBee network (Sensor to Nursing Station)</t>
+  </si>
+  <si>
+    <t>Fieldname</t>
+  </si>
+  <si>
+    <t>PatientAccountNo</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>BloodType</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Integer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
@@ -1134,37 +1167,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="107.85546875" style="10" customWidth="1"/>
+    <col min="1" max="1" width="107.83203125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="67.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" ht="32" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="105" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" ht="84" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="118.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:1" ht="147" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:1" ht="126" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>130</v>
       </c>
@@ -1177,614 +1210,668 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B86" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A102" sqref="A102"/>
+      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24" style="3" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="3" width="32.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="48" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="36" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="36" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="24" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="F36" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A70" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="E77" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="E78" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="D89" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A95" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="D99" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A102" s="1" t="s">
         <v>184</v>
       </c>
@@ -1803,17 +1890,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="117.5703125" customWidth="1"/>
+    <col min="1" max="1" width="117.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="383.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="383.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>88</v>
       </c>
@@ -1831,136 +1918,136 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.5703125" customWidth="1"/>
-    <col min="2" max="2" width="62.140625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="45.5" customWidth="1"/>
+    <col min="2" max="2" width="62.1640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="10" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" s="10" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" s="22" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="22"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" s="10" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="B22" s="10" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" s="10" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" s="10" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" s="10" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" s="10" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="B28" s="10" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="10" t="s">
         <v>155</v>
       </c>
@@ -1981,13 +2068,13 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54.140625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="54.1640625" style="10" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>77</v>
       </c>
@@ -1995,13 +2082,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>74</v>
       </c>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>75</v>
       </c>
@@ -2009,7 +2096,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>81</v>
       </c>
@@ -2017,7 +2104,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>84</v>
       </c>
@@ -2025,7 +2112,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>86</v>
       </c>
@@ -2033,17 +2120,17 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="14"/>
     </row>
-    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>79</v>
       </c>
       <c r="B8" s="14"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
     </row>
@@ -2060,14 +2147,14 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="24"/>
-    <col min="2" max="2" width="17.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="92.7109375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="24"/>
+    <col min="2" max="2" width="17.5" style="7" customWidth="1"/>
+    <col min="3" max="3" width="92.6640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>173</v>
       </c>
@@ -2078,7 +2165,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="24">
         <v>0.1</v>
       </c>
@@ -2089,7 +2176,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="24">
         <v>1</v>
       </c>
@@ -2100,7 +2187,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="24">
         <v>1.1000000000000001</v>
       </c>
@@ -2111,7 +2198,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="24">
         <v>1.2</v>
       </c>
@@ -2136,67 +2223,67 @@
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="114.28515625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="114.33203125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="75.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>172</v>
       </c>

</xml_diff>

<commit_message>
add better fields for spreadsheet
</commit_message>
<xml_diff>
--- a/services/health/cloud-mesh-security-use-case-table.xlsx
+++ b/services/health/cloud-mesh-security-use-case-table.xlsx
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="194">
-  <si>
-    <t>Object</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="199">
   <si>
     <t>First name</t>
   </si>
@@ -618,6 +615,24 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Example Property Value</t>
+  </si>
+  <si>
+    <t>Gregor</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>von Laszewski</t>
   </si>
 </sst>
 </file>
@@ -1178,28 +1193,28 @@
   <sheetData>
     <row r="1" spans="1:1" ht="32" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="84" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:1" ht="126" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1210,673 +1225,703 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="32.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24" style="3" customWidth="1"/>
-    <col min="6" max="6" width="23.5" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="27.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24" style="3" customWidth="1"/>
+    <col min="7" max="7" width="23.5" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>0</v>
+        <v>193</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>191</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>20</v>
+        <v>194</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+        <v>19</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1234</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="A27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="F27" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="24" x14ac:dyDescent="0.15">
+      <c r="A33" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="36" x14ac:dyDescent="0.15">
-      <c r="A21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="24" x14ac:dyDescent="0.15">
-      <c r="A27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A33" s="1" t="s">
+      <c r="F33" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="G36" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A37" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A38" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A37" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:7" ht="24" x14ac:dyDescent="0.15">
+      <c r="A39" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E39" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A40" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A39" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A40" s="1" t="s">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A41" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A41" s="1" t="s">
+      <c r="E41" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A42" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D42" s="1" t="s">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A43" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A43" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="E43" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A48" s="1" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A48" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A65" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A65" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A67" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A70" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A72" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A73" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A74" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A75" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A76" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="1" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A77" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A77" s="1" t="s">
+      <c r="F77" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A78" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E77" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A78" s="1" t="s">
+      <c r="F78" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E78" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A81" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A82" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A82" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A85" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A87" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A88" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A89" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A89" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D89" s="1" t="s">
+      <c r="E89" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A90" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A91" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A92" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A93" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A93" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A95" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A97" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A97" s="1" t="s">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A98" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A98" s="1" t="s">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A99" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A99" s="1" t="s">
+      <c r="E99" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A100" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="E100" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A100" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D100" s="1" t="s">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A101" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A101" s="1" t="s">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A102" s="1" t="s">
         <v>183</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A102" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1900,12 +1945,12 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="383.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1929,47 +1974,47 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1977,82 +2022,82 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="B22" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="B28" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2079,48 +2124,48 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="14"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>81</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>86</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2129,7 +2174,7 @@
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="14"/>
     </row>
@@ -2159,13 +2204,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2176,7 +2221,7 @@
         <v>43211</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2187,7 +2232,7 @@
         <v>43220</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2198,7 +2243,7 @@
         <v>43225</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2209,7 +2254,7 @@
         <v>43263</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2233,62 +2278,62 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>